<commit_message>
data: delete "parameters" tab from testing_data.xlsx
</commit_message>
<xml_diff>
--- a/test_mip_start/data/testing_data.xlsx
+++ b/test_mip_start/data/testing_data.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="parameters" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="foods" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="nutrients" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="foods_nutrients" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="foods" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="nutrients" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="foods_nutrients" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,19 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="41">
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food Cost Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Limit</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="37">
   <si>
     <t xml:space="preserve">Food ID</t>
   </si>
@@ -247,12 +234,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -471,211 +458,159 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.95"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D1010"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="14.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>2.49</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>2.89</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>1.5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>1.89</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>2.09</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>1.99</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>2.49</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>0.89</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>1.59</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3695,14 +3630,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -3715,25 +3650,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1800</v>
@@ -3744,10 +3679,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>91</v>
@@ -3755,10 +3690,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>0</v>
@@ -3769,10 +3704,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0</v>
@@ -3792,15 +3727,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3813,34 +3748,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>410</v>
@@ -3848,16 +3783,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>420</v>
@@ -3865,16 +3800,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E4" s="8" t="n">
         <v>560</v>
@@ -3882,16 +3817,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>380</v>
@@ -3899,16 +3834,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8" t="n">
         <v>320</v>
@@ -3916,16 +3851,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E7" s="8" t="n">
         <v>320</v>
@@ -3933,16 +3868,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8" t="n">
         <v>320</v>
@@ -3950,16 +3885,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="8" t="n">
         <v>100</v>
@@ -3967,16 +3902,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>330</v>
@@ -3984,16 +3919,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>24</v>
@@ -4001,16 +3936,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E12" s="8" t="n">
         <v>32</v>
@@ -4018,16 +3953,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>20</v>
@@ -4035,16 +3970,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E14" s="8" t="n">
         <v>4</v>
@@ -4052,16 +3987,16 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>12</v>
@@ -4069,16 +4004,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E16" s="8" t="n">
         <v>15</v>
@@ -4086,16 +4021,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E17" s="8" t="n">
         <v>31</v>
@@ -4103,16 +4038,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>8</v>
@@ -4120,16 +4055,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>8</v>
@@ -4137,16 +4072,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>26</v>
@@ -4154,16 +4089,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E21" s="8" t="n">
         <v>10</v>
@@ -4171,16 +4106,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E22" s="8" t="n">
         <v>32</v>
@@ -4188,16 +4123,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E23" s="8" t="n">
         <v>19</v>
@@ -4205,16 +4140,16 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E24" s="8" t="n">
         <v>10</v>
@@ -4222,16 +4157,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E25" s="8" t="n">
         <v>12</v>
@@ -4239,16 +4174,16 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E26" s="8" t="n">
         <v>12</v>
@@ -4256,16 +4191,16 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E27" s="8" t="n">
         <v>2.5</v>
@@ -4273,16 +4208,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E28" s="8" t="n">
         <v>10</v>
@@ -4290,16 +4225,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E29" s="8" t="n">
         <v>730</v>
@@ -4307,16 +4242,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E30" s="8" t="n">
         <v>1190</v>
@@ -4324,16 +4259,16 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E31" s="8" t="n">
         <v>1800</v>
@@ -4341,16 +4276,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E32" s="8" t="n">
         <v>270</v>
@@ -4358,16 +4293,16 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E33" s="8" t="n">
         <v>930</v>
@@ -4375,16 +4310,16 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E34" s="8" t="n">
         <v>820</v>
@@ -4392,16 +4327,16 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E35" s="8" t="n">
         <v>1230</v>
@@ -4409,16 +4344,16 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E36" s="8" t="n">
         <v>125</v>
@@ -4426,16 +4361,16 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E37" s="8" t="n">
         <v>180</v>

</xml_diff>

<commit_message>
data: testing_data.xlsx: rename Hamburguer -> Egg
</commit_message>
<xml_diff>
--- a/test_mip_start/data/testing_data.xlsx
+++ b/test_mip_start/data/testing_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="foods" sheetId="1" state="visible" r:id="rId3"/>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">F0</t>
   </si>
   <si>
-    <t xml:space="preserve">Hamburger</t>
+    <t xml:space="preserve">Egg</t>
   </si>
   <si>
     <t xml:space="preserve">F1</t>
@@ -447,8 +447,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,8 +684,8 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>